<commit_message>
iPad synth version finished
</commit_message>
<xml_diff>
--- a/BOM - orders/Order-2018-09-19/noisebox-order-20180919.xlsx
+++ b/BOM - orders/Order-2018-09-19/noisebox-order-20180919.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnnyvenom/Documents/Projects/Noisebox-2018/BOM - orders/Order-2018-09-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260B26BF-5DE3-0F4E-BE5C-D6EE93D11449}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE84CA98-9329-7549-A9AC-A2183D5590C4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11420" yWindow="-28940" windowWidth="28240" windowHeight="24420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,9 +107,6 @@
     <t>Adafruit</t>
   </si>
   <si>
-    <t>Battery LiPo 660mA</t>
-  </si>
-  <si>
     <t>https://www.adafruit.com/product/2465</t>
   </si>
   <si>
@@ -261,6 +258,9 @@
   </si>
   <si>
     <t>New Noisebox 1st prototypes</t>
+  </si>
+  <si>
+    <t>Battery LiPo 6600mA</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1031,7 @@
   <dimension ref="A1:S57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1051,10 +1051,10 @@
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
@@ -1113,16 +1113,16 @@
     </row>
     <row r="4" spans="1:19" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="68" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C4" s="52">
         <v>2465</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" s="55" t="s">
         <v>11</v>
@@ -1132,7 +1132,7 @@
       </c>
       <c r="G4" s="49">
         <f>A4*F4</f>
-        <v>29.5</v>
+        <v>59</v>
       </c>
       <c r="H4" s="50"/>
       <c r="J4" s="48"/>
@@ -1148,16 +1148,16 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="52">
         <v>353</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" s="55" t="s">
         <v>11</v>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="G5" s="49">
         <f t="shared" ref="G5:G11" si="0">A5*F5</f>
-        <v>19.95</v>
+        <v>39.9</v>
       </c>
       <c r="H5" s="10"/>
       <c r="J5" s="2"/>
@@ -1186,13 +1186,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="74">
         <v>2225</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="55" t="s">
         <v>11</v>
@@ -1218,16 +1218,16 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7" s="68" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="52">
         <v>3581</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E7" s="55" t="s">
         <v>11</v>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="G7" s="49">
         <f>A7*F7</f>
-        <v>13.9</v>
+        <v>27.8</v>
       </c>
       <c r="H7" s="10"/>
       <c r="J7" s="2"/>
@@ -1256,13 +1256,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="68" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="52">
         <v>559</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="55" t="s">
         <v>11</v>
@@ -1291,13 +1291,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="52">
         <v>1505</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="55" t="s">
         <v>11</v>
@@ -1326,13 +1326,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="68" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="52">
         <v>1445</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="55" t="s">
         <v>11</v>
@@ -1361,13 +1361,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="68" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="74">
         <v>2046</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="55" t="s">
         <v>11</v>
@@ -1393,16 +1393,16 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" s="68" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="52">
         <v>1994</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="55" t="s">
         <v>11</v>
@@ -1412,7 +1412,7 @@
       </c>
       <c r="G12" s="49">
         <f>A12*F12</f>
-        <v>6.95</v>
+        <v>13.9</v>
       </c>
       <c r="H12" s="10"/>
       <c r="J12" s="2"/>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="G13" s="49">
         <f>SUM(G4:G12)</f>
-        <v>108.7</v>
+        <v>179</v>
       </c>
       <c r="H13" s="10"/>
       <c r="J13" s="2"/>
@@ -1458,7 +1458,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="53"/>
       <c r="F14" s="56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G14" s="58">
         <v>16.989999999999998</v>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="G16" s="49">
         <f>SUM(G13:G15)</f>
-        <v>144.71</v>
+        <v>215.01000000000002</v>
       </c>
       <c r="H16" s="10"/>
     </row>
@@ -1498,7 +1498,6 @@
       <c r="A17" s="30"/>
       <c r="B17" s="25"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
       <c r="E17" s="15"/>
       <c r="F17" s="57" t="s">
         <v>14</v>
@@ -1519,13 +1518,13 @@
       </c>
       <c r="G18" s="60">
         <f>G16*G17</f>
-        <v>187.732283</v>
+        <v>278.93247300000002</v>
       </c>
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1540,13 +1539,13 @@
         <v>10</v>
       </c>
       <c r="B20" s="68" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="55" t="s">
         <v>16</v>
@@ -1565,13 +1564,13 @@
         <v>10</v>
       </c>
       <c r="B21" s="68" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="55" t="s">
         <v>16</v>
@@ -1590,13 +1589,13 @@
         <v>10</v>
       </c>
       <c r="B22" s="68" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="76" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="55" t="s">
         <v>16</v>
@@ -1615,13 +1614,13 @@
         <v>3</v>
       </c>
       <c r="B23" s="75" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E23" s="55" t="s">
         <v>16</v>
@@ -1640,13 +1639,13 @@
         <v>3</v>
       </c>
       <c r="B24" s="75" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" s="55" t="s">
         <v>16</v>
@@ -1665,13 +1664,13 @@
         <v>1</v>
       </c>
       <c r="B25" s="75" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" s="55" t="s">
         <v>16</v>
@@ -1690,13 +1689,13 @@
         <v>2</v>
       </c>
       <c r="B26" s="75" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" s="55" t="s">
         <v>16</v>
@@ -1712,16 +1711,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="45" t="s">
+      <c r="D27" s="38" t="s">
         <v>62</v>
-      </c>
-      <c r="D27" s="38" t="s">
-        <v>63</v>
       </c>
       <c r="E27" s="55" t="s">
         <v>16</v>
@@ -1731,22 +1730,22 @@
       </c>
       <c r="G27" s="49">
         <f t="shared" si="1"/>
-        <v>20.63</v>
+        <v>41.26</v>
       </c>
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B28" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="45" t="s">
+      <c r="D28" s="38" t="s">
         <v>65</v>
-      </c>
-      <c r="D28" s="38" t="s">
-        <v>66</v>
       </c>
       <c r="E28" s="55" t="s">
         <v>16</v>
@@ -1756,7 +1755,7 @@
       </c>
       <c r="G28" s="49">
         <f t="shared" si="1"/>
-        <v>6.83</v>
+        <v>13.66</v>
       </c>
       <c r="H28" s="10"/>
     </row>
@@ -1771,7 +1770,7 @@
       </c>
       <c r="G29" s="49">
         <f>SUM(G20:G28)</f>
-        <v>105.22</v>
+        <v>132.68</v>
       </c>
       <c r="H29" s="10"/>
     </row>
@@ -1791,7 +1790,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="77" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1810,7 +1809,7 @@
         <v>17</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1821,10 +1820,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="79" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -1834,7 +1833,7 @@
       </c>
       <c r="G33" s="70">
         <f>SUM(G29,G31,G32)</f>
-        <v>110.48</v>
+        <v>137.94</v>
       </c>
       <c r="H33" s="12"/>
     </row>
@@ -1920,7 +1919,7 @@
       </c>
       <c r="G40" s="29">
         <f>SUM(G18,G33)</f>
-        <v>298.21228300000001</v>
+        <v>416.87247300000001</v>
       </c>
       <c r="H40" s="21"/>
     </row>
@@ -1930,25 +1929,25 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{E0019E62-E868-E74E-96D0-56F21A5EC6CD}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{27B52E8B-9E45-1B48-9284-954DA3CDFF2B}"/>
-    <hyperlink ref="D12" r:id="rId3" xr:uid="{FD41DB75-50FF-5146-92F2-512170CF03AD}"/>
-    <hyperlink ref="D9" r:id="rId4" xr:uid="{748D494B-C194-154D-8569-A2CF3C61DEEB}"/>
-    <hyperlink ref="D10" r:id="rId5" xr:uid="{DE54B882-E219-D543-B9D1-46D6551EE9FD}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{2E1C1EB7-F64D-D348-A896-9801AB79E456}"/>
-    <hyperlink ref="D6" r:id="rId7" xr:uid="{323B5386-F544-6944-A320-3EE5CFE82973}"/>
-    <hyperlink ref="D11" r:id="rId8" xr:uid="{E00BFBDD-3C73-1346-AC7E-CF27289818F3}"/>
-    <hyperlink ref="C23" r:id="rId9" xr:uid="{968E03CF-5920-8C4A-9C35-C55622DD38E4}"/>
-    <hyperlink ref="C24" r:id="rId10" xr:uid="{62125BFB-64C4-9E4C-A9B7-8C4621E1B6FD}"/>
-    <hyperlink ref="C26" r:id="rId11" xr:uid="{97F7E648-B1AD-E649-82A5-F330E680B62B}"/>
-    <hyperlink ref="C20" r:id="rId12" display="P160KNP-0QC20A10K" xr:uid="{DD53DDFE-2126-D441-873A-373CC63ED224}"/>
-    <hyperlink ref="C21" r:id="rId13" display="485-1988" xr:uid="{971F337B-3642-7244-806D-C9F2B2466598}"/>
-    <hyperlink ref="C22" r:id="rId14" xr:uid="{60157030-E412-1B49-B184-B521E4D7A04B}"/>
-    <hyperlink ref="C25" r:id="rId15" xr:uid="{69990502-377F-0A45-AC7F-3D353FBAA912}"/>
-    <hyperlink ref="C27" r:id="rId16" xr:uid="{FCBFFB55-F5AD-8E41-A15E-A8434350997F}"/>
-    <hyperlink ref="C28" r:id="rId17" xr:uid="{23562FC4-A310-8E45-B419-7CE0950DBB2E}"/>
-    <hyperlink ref="B33" r:id="rId18" xr:uid="{891B5824-103F-EE42-A318-3389512A7AA8}"/>
-    <hyperlink ref="D7" r:id="rId19" xr:uid="{D0540513-A585-B04B-8BBE-26D4DE66ED2B}"/>
+    <hyperlink ref="D12" r:id="rId1" xr:uid="{FD41DB75-50FF-5146-92F2-512170CF03AD}"/>
+    <hyperlink ref="D9" r:id="rId2" xr:uid="{748D494B-C194-154D-8569-A2CF3C61DEEB}"/>
+    <hyperlink ref="D10" r:id="rId3" xr:uid="{DE54B882-E219-D543-B9D1-46D6551EE9FD}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{2E1C1EB7-F64D-D348-A896-9801AB79E456}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{323B5386-F544-6944-A320-3EE5CFE82973}"/>
+    <hyperlink ref="D11" r:id="rId6" xr:uid="{E00BFBDD-3C73-1346-AC7E-CF27289818F3}"/>
+    <hyperlink ref="C23" r:id="rId7" xr:uid="{968E03CF-5920-8C4A-9C35-C55622DD38E4}"/>
+    <hyperlink ref="C24" r:id="rId8" xr:uid="{62125BFB-64C4-9E4C-A9B7-8C4621E1B6FD}"/>
+    <hyperlink ref="C26" r:id="rId9" xr:uid="{97F7E648-B1AD-E649-82A5-F330E680B62B}"/>
+    <hyperlink ref="C20" r:id="rId10" display="P160KNP-0QC20A10K" xr:uid="{DD53DDFE-2126-D441-873A-373CC63ED224}"/>
+    <hyperlink ref="C21" r:id="rId11" display="485-1988" xr:uid="{971F337B-3642-7244-806D-C9F2B2466598}"/>
+    <hyperlink ref="C22" r:id="rId12" xr:uid="{60157030-E412-1B49-B184-B521E4D7A04B}"/>
+    <hyperlink ref="C25" r:id="rId13" xr:uid="{69990502-377F-0A45-AC7F-3D353FBAA912}"/>
+    <hyperlink ref="C27" r:id="rId14" xr:uid="{FCBFFB55-F5AD-8E41-A15E-A8434350997F}"/>
+    <hyperlink ref="C28" r:id="rId15" xr:uid="{23562FC4-A310-8E45-B419-7CE0950DBB2E}"/>
+    <hyperlink ref="B33" r:id="rId16" xr:uid="{891B5824-103F-EE42-A318-3389512A7AA8}"/>
+    <hyperlink ref="D7" r:id="rId17" xr:uid="{D0540513-A585-B04B-8BBE-26D4DE66ED2B}"/>
+    <hyperlink ref="D4" r:id="rId18" xr:uid="{E7217F95-A556-9F44-B55C-5706E07F21E7}"/>
+    <hyperlink ref="D5" r:id="rId19" xr:uid="{14D3FBEB-5116-1B41-8436-3E0E13D5CFB0}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>